<commit_message>
Despues de las pruebas de Agaela
</commit_message>
<xml_diff>
--- a/tableros/tableros.xlsx
+++ b/tableros/tableros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udcgal-my.sharepoint.com/personal/pablo_paramo_telle_udc_es/Documents/UDC4/TFG/ComunicELA-tfg/tableros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="378" documentId="11_F25DC773A252ABDACC1048B8A15C52B85ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68D0126D-3541-4032-96BB-A4F6CDB26E5F}"/>
+  <xr:revisionPtr revIDLastSave="479" documentId="11_F25DC773A252ABDACC1048B8A15C52B85ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86661EC8-701A-48B1-9AD1-0ABA6CD5B3D2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inicial" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="149">
   <si>
     <t>TAB. VERBOS</t>
   </si>
@@ -88,12 +88,6 @@
     <t>VER</t>
   </si>
   <si>
-    <t>OLER</t>
-  </si>
-  <si>
-    <t>ESTAR</t>
-  </si>
-  <si>
     <t>TENER</t>
   </si>
   <si>
@@ -124,9 +118,6 @@
     <t>PENSAR</t>
   </si>
   <si>
-    <t>DISCUTIR</t>
-  </si>
-  <si>
     <t>ABRIR</t>
   </si>
   <si>
@@ -136,18 +127,6 @@
     <t>LLEVAR</t>
   </si>
   <si>
-    <t>COMPRAR</t>
-  </si>
-  <si>
-    <t>VESTIR</t>
-  </si>
-  <si>
-    <t>VENIR</t>
-  </si>
-  <si>
-    <t>TRAER</t>
-  </si>
-  <si>
     <t>AYUDA</t>
   </si>
   <si>
@@ -163,18 +142,9 @@
     <t>MAL</t>
   </si>
   <si>
-    <t>MENOS</t>
-  </si>
-  <si>
     <t>TÚ</t>
   </si>
   <si>
-    <t>ABUELO</t>
-  </si>
-  <si>
-    <t>ABUELA</t>
-  </si>
-  <si>
     <t>PADRE</t>
   </si>
   <si>
@@ -214,18 +184,6 @@
     <t>POLLO</t>
   </si>
   <si>
-    <t>HUEVO</t>
-  </si>
-  <si>
-    <t>TORTILLA</t>
-  </si>
-  <si>
-    <t>ALBONDIGAS</t>
-  </si>
-  <si>
-    <t>CROQUETAS</t>
-  </si>
-  <si>
     <t>PIZZA</t>
   </si>
   <si>
@@ -253,9 +211,6 @@
     <t>MANZANA</t>
   </si>
   <si>
-    <t>CHOCOLATE</t>
-  </si>
-  <si>
     <t>LECHUGA</t>
   </si>
   <si>
@@ -280,18 +235,6 @@
     <t>HORNO</t>
   </si>
   <si>
-    <t>ESTUFA</t>
-  </si>
-  <si>
-    <t>VENTILADOR</t>
-  </si>
-  <si>
-    <t>PAPELERA</t>
-  </si>
-  <si>
-    <t>JUGUETE</t>
-  </si>
-  <si>
     <t>CASA</t>
   </si>
   <si>
@@ -325,30 +268,15 @@
     <t>MUSEO</t>
   </si>
   <si>
-    <t>HOTEL</t>
-  </si>
-  <si>
-    <t>MONTAÑA</t>
-  </si>
-  <si>
-    <t>PLAYA</t>
-  </si>
-  <si>
     <t>AMBULANCIA</t>
   </si>
   <si>
     <t>COCHE</t>
   </si>
   <si>
-    <t>CAMIÓN</t>
-  </si>
-  <si>
     <t>TAXI</t>
   </si>
   <si>
-    <t>TRACTOR</t>
-  </si>
-  <si>
     <t>BICICLETA</t>
   </si>
   <si>
@@ -361,9 +289,6 @@
     <t>BARCO</t>
   </si>
   <si>
-    <t>COHETE</t>
-  </si>
-  <si>
     <t>METRO</t>
   </si>
   <si>
@@ -388,15 +313,6 @@
     <t>LLAVE</t>
   </si>
   <si>
-    <t>DUCHA</t>
-  </si>
-  <si>
-    <t>VASO</t>
-  </si>
-  <si>
-    <t>PLATO</t>
-  </si>
-  <si>
     <t>PERRO</t>
   </si>
   <si>
@@ -427,9 +343,6 @@
     <t>CABEZA</t>
   </si>
   <si>
-    <t>PELO</t>
-  </si>
-  <si>
     <t>NARIZ</t>
   </si>
   <si>
@@ -445,21 +358,12 @@
     <t>CUELLO</t>
   </si>
   <si>
-    <t>HOMBRO</t>
-  </si>
-  <si>
     <t>BRAZO</t>
   </si>
   <si>
-    <t>PECHO</t>
-  </si>
-  <si>
     <t>MANO</t>
   </si>
   <si>
-    <t>CINTURA</t>
-  </si>
-  <si>
     <t>PIERNA</t>
   </si>
   <si>
@@ -502,36 +406,15 @@
     <t>LEJOS</t>
   </si>
   <si>
-    <t>LLENO</t>
-  </si>
-  <si>
     <t>DESPUÉS</t>
   </si>
   <si>
-    <t>GRANJA</t>
-  </si>
-  <si>
-    <t>MAR</t>
-  </si>
-  <si>
-    <t>BOSQUE</t>
-  </si>
-  <si>
-    <t>RIO</t>
-  </si>
-  <si>
     <t>PARA</t>
   </si>
   <si>
     <t>PODER</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>PRIMERO</t>
-  </si>
-  <si>
     <t>BOTELLA</t>
   </si>
   <si>
@@ -541,9 +424,6 @@
     <t>TAB. RÁPIDO</t>
   </si>
   <si>
-    <t>MÁS</t>
-  </si>
-  <si>
     <t>PURÉ</t>
   </si>
   <si>
@@ -556,21 +436,12 @@
     <t>TELEVISIÓN</t>
   </si>
   <si>
-    <t>POLICÍA</t>
-  </si>
-  <si>
-    <t>JARDÍN</t>
-  </si>
-  <si>
     <t>AUTOBÚS</t>
   </si>
   <si>
     <t>AVIÓN</t>
   </si>
   <si>
-    <t>HELICÓPTERO</t>
-  </si>
-  <si>
     <t>HABITACIÓN</t>
   </si>
   <si>
@@ -580,33 +451,15 @@
     <t>SOFÁ</t>
   </si>
   <si>
-    <t>LÁMPARA</t>
-  </si>
-  <si>
     <t>PÁJARO</t>
   </si>
   <si>
     <t>DELFÍN</t>
   </si>
   <si>
-    <t>VACÍO</t>
-  </si>
-  <si>
-    <t>ÚLTIMO</t>
-  </si>
-  <si>
     <t>SÍ</t>
   </si>
   <si>
-    <t>PLÁTANO</t>
-  </si>
-  <si>
-    <t>MELÓN</t>
-  </si>
-  <si>
-    <t>YOGUR</t>
-  </si>
-  <si>
     <t>EL-ELLA</t>
   </si>
   <si>
@@ -614,9 +467,6 @@
   </si>
   <si>
     <t>AMIGO-A</t>
-  </si>
-  <si>
-    <t>VECINO-A</t>
   </si>
   <si>
     <t>NOSOTROS-AS</t>
@@ -972,7 +822,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>166</v>
+        <v>127</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1006,7 +856,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -1019,10 +869,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA552ACA-96DE-4E53-B417-0ACC75AB62BE}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1037,55 +887,41 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>195</v>
+        <v>145</v>
       </c>
       <c r="D1" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>175</v>
-      </c>
-      <c r="B4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1095,10 +931,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A50E60F1-2F1E-4687-9D5F-1A293A57DF1A}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1111,55 +947,41 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
-        <v>177</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>180</v>
-      </c>
-      <c r="B4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1169,10 +991,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F704A5E-771D-4BE2-BF1A-D1D2849EFCC4}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1188,55 +1010,41 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="D1" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>181</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>156</v>
-      </c>
-      <c r="B4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D4" t="s">
-        <v>158</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1246,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D039E4-E987-4221-9983-5576BB2B2ABE}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1262,55 +1070,41 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="C1" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="D1" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1320,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0BAF42D-658C-4F53-B46F-DDD16A5FEECB}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1337,55 +1131,41 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
       <c r="D1" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="D2" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B4" t="s">
-        <v>183</v>
-      </c>
-      <c r="C4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D4" t="s">
-        <v>184</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1395,10 +1175,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A62245C-7216-4E59-A7A6-EB1025A979B4}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1414,55 +1194,41 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>123</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>167</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>162</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1472,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180B4D93-F365-4E8C-A6A5-9CB56BB5C688}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1493,7 +1259,7 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>13</v>
@@ -1501,44 +1267,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>198</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1548,10 +1300,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F46D395-647B-499E-A681-BED4D69A129D}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1570,52 +1322,38 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
         <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1625,10 +1363,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D5383A-5161-4D33-96CC-18EDADC3FD94}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1644,55 +1382,41 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1702,10 +1426,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD2A1F31-2A4A-483F-91F0-B344C7ED283F}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1724,52 +1448,38 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>169</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>186</v>
-      </c>
-      <c r="B4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1779,10 +1489,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD4D96E3-BE9A-4FD1-B927-4EA58545D53E}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1798,55 +1508,41 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>170</v>
+        <v>130</v>
       </c>
       <c r="D1" t="s">
-        <v>165</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>164</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1856,10 +1552,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F640BD6F-CC6B-4C43-BDF1-90158D4567BF}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1875,55 +1571,41 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="D1" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
-        <v>190</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>172</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" t="s">
-        <v>192</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1933,10 +1615,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7304D0-8C5B-4882-9055-C507E06966D8}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1951,55 +1633,41 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" t="s">
-        <v>173</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>